<commit_message>
(ABM-777) Update input_truck directory zone references for port and airport freight
</commit_message>
<xml_diff>
--- a/input_truck/regionaltrips2010-2015.xlsx
+++ b/input_truck/regionaltrips2010-2015.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\apps\ABM_develop\input_truck\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="19035" windowHeight="11760"/>
   </bookViews>
@@ -17,7 +22,7 @@
     <sheet name="regionalEEtrips2010" sheetId="10" r:id="rId8"/>
     <sheet name="regionalEEtrips2015" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -42,9 +47,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -76,7 +81,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -86,6 +91,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -134,7 +142,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -167,9 +175,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -202,6 +227,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -378,10 +420,393 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>2010</v>
+      </c>
+      <c r="C1">
+        <v>2011</v>
+      </c>
+      <c r="D1">
+        <v>2012</v>
+      </c>
+      <c r="E1">
+        <v>2013</v>
+      </c>
+      <c r="F1">
+        <v>2014</v>
+      </c>
+      <c r="G1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3789.28</v>
+      </c>
+      <c r="C2" s="1">
+        <f>$B2+($G2-$B2)/($G$1-$B$1)*(C$1-$B$1)</f>
+        <v>3847.4780000000001</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:F2" si="0">$B2+($G2-$B2)/($G$1-$B$1)*(D$1-$B$1)</f>
+        <v>3905.6759999999999</v>
+      </c>
+      <c r="E2" s="1">
+        <f t="shared" si="0"/>
+        <v>3963.8740000000003</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" si="0"/>
+        <v>4022.0720000000001</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4080.27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>4525</v>
+      </c>
+      <c r="B3" s="1">
+        <v>202.67</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:F8" si="1">$B3+($G3-$B3)/($G$1-$B$1)*(C$1-$B$1)</f>
+        <v>211.67999999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="1"/>
+        <v>220.69</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" si="1"/>
+        <v>229.7</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="1"/>
+        <v>238.70999999999998</v>
+      </c>
+      <c r="G3" s="1">
+        <v>247.72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3798</v>
+      </c>
+      <c r="B4" s="1">
+        <v>202.67</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="1"/>
+        <v>211.67999999999998</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="1"/>
+        <v>220.69</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="1"/>
+        <v>229.7</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="1"/>
+        <v>238.70999999999998</v>
+      </c>
+      <c r="G4" s="1">
+        <v>247.72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1569.3100999999999</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="1"/>
+        <v>1598.62408</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="1"/>
+        <v>1627.93806</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>1657.2520400000001</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>1686.56602</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1715.88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>436.72</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="1"/>
+        <v>449.69200000000001</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="1"/>
+        <v>462.66399999999999</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>475.63599999999997</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>488.608</v>
+      </c>
+      <c r="G6" s="1">
+        <v>501.58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1613.54</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="1"/>
+        <v>1757.2239999999999</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="1"/>
+        <v>1900.9079999999999</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>2044.5920000000001</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>2188.2759999999998</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2331.96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3668</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.22</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="1"/>
+        <v>1.31</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>1.49</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>1.58</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1.67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>3789.28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>1569.3100999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>436.72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1613.54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3668</v>
+      </c>
+      <c r="B6">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4525</v>
+      </c>
+      <c r="B7" s="1">
+        <v>202.67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3798</v>
+      </c>
+      <c r="B8" s="1">
+        <v>202.67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>4080.27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>1715.88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>501.58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>2331.96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3668</v>
+      </c>
+      <c r="B6">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4525</v>
+      </c>
+      <c r="B7" s="1">
+        <v>247.72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3798</v>
+      </c>
+      <c r="B8" s="1">
+        <v>247.72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -414,502 +839,187 @@
         <v>12</v>
       </c>
       <c r="B2" s="1">
-        <v>3789.28</v>
+        <v>2525.4299000000001</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2:D2" si="0">$B2+($G2-$B2)/($G1-$B1)*(C1-$B1)</f>
-        <v>3847.4780000000001</v>
+        <f>$B2+($G2-$B2)/($G$1-$B$1)*(C$1-$B$1)</f>
+        <v>2694.9259000000002</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" si="0"/>
-        <v>3905.6759999999999</v>
+        <f t="shared" ref="D2:F8" si="0">$B2+($G2-$B2)/($G$1-$B$1)*(D$1-$B$1)</f>
+        <v>2864.4219000000003</v>
       </c>
       <c r="E2" s="1">
-        <f>$B2+($G2-$B2)/($G1-$B1)*(E1-$B1)</f>
-        <v>3963.8740000000003</v>
+        <f t="shared" si="0"/>
+        <v>3033.9179000000004</v>
       </c>
       <c r="F2" s="1">
-        <f>$B2+($G2-$B2)/($G1-$B1)*(F1-$B1)</f>
-        <v>4022.0720000000001</v>
+        <f t="shared" si="0"/>
+        <v>3203.4139</v>
       </c>
       <c r="G2" s="1">
-        <v>4080.27</v>
+        <v>3372.9099000000001</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>4179</v>
+        <v>4525</v>
       </c>
       <c r="B3" s="1">
-        <v>405.34</v>
+        <v>7.72</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C7" si="1">$B3+($G3-$B3)/($G2-$B2)*(C2-$B2)</f>
-        <v>423.35999999999996</v>
+        <f t="shared" ref="C3:C8" si="1">$B3+($G3-$B3)/($G$1-$B$1)*(C$1-$B$1)</f>
+        <v>8.0190000000000001</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D7" si="2">$B3+($G3-$B3)/($G2-$B2)*(D2-$B2)</f>
-        <v>441.37999999999994</v>
+        <f t="shared" si="0"/>
+        <v>8.3179999999999996</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E7" si="3">$B3+($G3-$B3)/($G2-$B2)*(E2-$B2)</f>
-        <v>459.40000000000003</v>
+        <f t="shared" si="0"/>
+        <v>8.6169999999999991</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F7" si="4">$B3+($G3-$B3)/($G2-$B2)*(F2-$B2)</f>
-        <v>477.42</v>
+        <f t="shared" si="0"/>
+        <v>8.9160000000000004</v>
       </c>
       <c r="G3" s="1">
-        <v>495.44</v>
+        <v>9.2149999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>10</v>
+        <v>3798</v>
       </c>
       <c r="B4" s="1">
-        <v>1569.3100999999999</v>
+        <v>7.72</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="1"/>
-        <v>1598.6240799999998</v>
+        <v>8.0190000000000001</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="2"/>
-        <v>1627.93806</v>
+        <f t="shared" si="0"/>
+        <v>8.3179999999999996</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="3"/>
-        <v>1657.2520400000001</v>
+        <f t="shared" si="0"/>
+        <v>8.6169999999999991</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="4"/>
-        <v>1686.5660200000002</v>
+        <f t="shared" si="0"/>
+        <v>8.9160000000000004</v>
       </c>
       <c r="G4" s="1">
-        <v>1715.88</v>
+        <v>9.2149999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>436.72</v>
+        <v>1052.8</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="1"/>
-        <v>449.69199999999995</v>
+        <v>1119.384</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="2"/>
-        <v>462.66399999999999</v>
+        <f t="shared" si="0"/>
+        <v>1185.9680000000001</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="3"/>
-        <v>475.63600000000002</v>
+        <f t="shared" si="0"/>
+        <v>1252.5520000000001</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="4"/>
-        <v>488.60800000000006</v>
+        <f t="shared" si="0"/>
+        <v>1319.136</v>
       </c>
       <c r="G5" s="1">
-        <v>501.58</v>
+        <v>1385.72</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>1613.54</v>
+        <v>309.56</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>1757.2239999999993</v>
+        <v>330.29399999999998</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="2"/>
-        <v>1900.9079999999997</v>
+        <f t="shared" si="0"/>
+        <v>351.02800000000002</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="3"/>
-        <v>2044.5920000000003</v>
+        <f t="shared" si="0"/>
+        <v>371.762</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="4"/>
-        <v>2188.2760000000007</v>
+        <f t="shared" si="0"/>
+        <v>392.49599999999998</v>
       </c>
       <c r="G6" s="1">
-        <v>2331.96</v>
+        <v>413.23</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3494</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1">
-        <v>1.22</v>
+        <v>1758.4</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="1"/>
-        <v>1.3099999999999996</v>
+        <v>1834.672</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="2"/>
-        <v>1.3999999999999997</v>
+        <f t="shared" si="0"/>
+        <v>1910.9440000000002</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="3"/>
-        <v>1.4900000000000002</v>
+        <f t="shared" si="0"/>
+        <v>1987.2160000000001</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="4"/>
-        <v>1.5800000000000005</v>
+        <f t="shared" si="0"/>
+        <v>2063.4880000000003</v>
       </c>
       <c r="G7" s="1">
-        <v>1.67</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>12</v>
-      </c>
-      <c r="B2">
-        <v>3789.28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>4179</v>
-      </c>
-      <c r="B3">
-        <v>405.34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>1569.3100999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>436.72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>1613.54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>3494</v>
-      </c>
-      <c r="B7">
-        <v>1.22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>12</v>
-      </c>
-      <c r="B2">
-        <v>4080.27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>4179</v>
-      </c>
-      <c r="B3">
-        <v>495.44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>1715.88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>501.58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>2331.96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>3494</v>
-      </c>
-      <c r="B7">
-        <v>1.67</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B1">
-        <v>2010</v>
-      </c>
-      <c r="C1">
-        <v>2011</v>
-      </c>
-      <c r="D1">
-        <v>2012</v>
-      </c>
-      <c r="E1">
-        <v>2013</v>
-      </c>
-      <c r="F1">
-        <v>2014</v>
-      </c>
-      <c r="G1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2525.4299000000001</v>
-      </c>
-      <c r="C2" s="1">
-        <f t="shared" ref="C2:F7" si="0">$B2+($G2-$B2)/($G1-$B1)*(C1-$B1)</f>
-        <v>2694.9259000000002</v>
-      </c>
-      <c r="D2" s="1">
-        <f t="shared" si="0"/>
-        <v>2864.4219000000003</v>
-      </c>
-      <c r="E2" s="1">
-        <f>$B2+($G2-$B2)/($G1-$B1)*(E1-$B1)</f>
-        <v>3033.9179000000004</v>
-      </c>
-      <c r="F2" s="1">
-        <f>$B2+($G2-$B2)/($G1-$B1)*(F1-$B1)</f>
-        <v>3203.4139</v>
-      </c>
-      <c r="G2" s="1">
-        <v>3372.9099000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>4179</v>
-      </c>
-      <c r="B3" s="1">
-        <v>15.44</v>
-      </c>
-      <c r="C3" s="1">
-        <f t="shared" si="0"/>
-        <v>16.038</v>
-      </c>
-      <c r="D3" s="1">
-        <f t="shared" si="0"/>
-        <v>16.635999999999999</v>
-      </c>
-      <c r="E3" s="1">
-        <f t="shared" si="0"/>
-        <v>17.234000000000002</v>
-      </c>
-      <c r="F3" s="1">
-        <f t="shared" si="0"/>
-        <v>17.832000000000001</v>
-      </c>
-      <c r="G3" s="1">
-        <v>18.43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1052.8</v>
-      </c>
-      <c r="C4" s="1">
-        <f t="shared" si="0"/>
-        <v>1119.384</v>
-      </c>
-      <c r="D4" s="1">
-        <f t="shared" si="0"/>
-        <v>1185.9679999999998</v>
-      </c>
-      <c r="E4" s="1">
-        <f t="shared" si="0"/>
-        <v>1252.5520000000001</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>1319.1360000000002</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1385.72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>309.56</v>
-      </c>
-      <c r="C5" s="1">
-        <f t="shared" si="0"/>
-        <v>330.29400000000004</v>
-      </c>
-      <c r="D5" s="1">
-        <f t="shared" si="0"/>
-        <v>351.02799999999996</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" si="0"/>
-        <v>371.76200000000006</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>392.49600000000009</v>
-      </c>
-      <c r="G5" s="1">
-        <v>413.23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1758.4</v>
-      </c>
-      <c r="C6" s="1">
-        <f t="shared" si="0"/>
-        <v>1834.6720000000003</v>
-      </c>
-      <c r="D6" s="1">
-        <f t="shared" si="0"/>
-        <v>1910.944</v>
-      </c>
-      <c r="E6" s="1">
-        <f t="shared" si="0"/>
-        <v>1987.2160000000003</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>2063.4880000000003</v>
-      </c>
-      <c r="G6" s="1">
         <v>2139.7600000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>3494</v>
-      </c>
-      <c r="B7" s="1">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3668</v>
+      </c>
+      <c r="B8" s="1">
         <v>0.95</v>
       </c>
-      <c r="C7" s="1">
-        <f t="shared" si="0"/>
+      <c r="C8" s="1">
+        <f t="shared" si="1"/>
         <v>0.99199999999999999</v>
       </c>
-      <c r="D7" s="1">
-        <f t="shared" si="0"/>
-        <v>1.0339999999999998</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.034</v>
+      </c>
+      <c r="E8" s="1">
         <f t="shared" si="0"/>
         <v>1.0760000000000001</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F8" s="1">
         <f t="shared" si="0"/>
         <v>1.1179999999999999</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G8" s="1">
         <v>1.1599999999999999</v>
       </c>
     </row>
@@ -920,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -946,42 +1056,50 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>4179</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>15.44</v>
+        <v>1052.8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>1052.8</v>
+        <v>309.56</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>309.56</v>
+        <v>1758.4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>3668</v>
       </c>
       <c r="B6">
-        <v>1758.4</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3494</v>
-      </c>
-      <c r="B7">
-        <v>0.95</v>
+        <v>4525</v>
+      </c>
+      <c r="B7" s="1">
+        <v>7.72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3798</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7.72</v>
       </c>
     </row>
   </sheetData>
@@ -991,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1017,42 +1135,50 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>4179</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>18.43</v>
+        <v>1385.72</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>1385.72</v>
+        <v>413.23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>413.23</v>
+        <v>2139.7600000000002</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>3668</v>
       </c>
       <c r="B6">
-        <v>2139.7600000000002</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3494</v>
-      </c>
-      <c r="B7">
-        <v>1.1599999999999999</v>
+        <v>4525</v>
+      </c>
+      <c r="B7" s="1">
+        <v>9.2149999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3798</v>
+      </c>
+      <c r="B8" s="1">
+        <v>9.2149999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1062,10 +1188,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E15"/>
+      <selection activeCell="H10" activeCellId="1" sqref="A10:B21 H10:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1106,29 +1232,29 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>4179</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1">
-        <v>9.8000000000000007</v>
+        <v>469.56</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:G7" si="0">$C2+($H2-$C2)/($H1-$C1)*(D1-$C1)</f>
-        <v>10.5</v>
+        <f t="shared" ref="D2:G21" si="0">$C2+($H2-$C2)/($H$1-$C$1)*(D$1-$C$1)</f>
+        <v>483.82799999999997</v>
       </c>
       <c r="E2" s="1">
-        <f t="shared" si="0"/>
-        <v>11.200000000000001</v>
+        <f t="shared" ref="E2:G11" si="1">$C2+($H2-$C2)/($H$1-$C$1)*(E$1-$C$1)</f>
+        <v>498.096</v>
       </c>
       <c r="F2" s="1">
-        <f>$C2+($H2-$C2)/($H1-$C1)*(F1-$C1)</f>
-        <v>11.9</v>
+        <f t="shared" si="1"/>
+        <v>512.36400000000003</v>
       </c>
       <c r="G2" s="1">
-        <f>$C2+($H2-$C2)/($H1-$C1)*(G1-$C1)</f>
-        <v>12.600000000000001</v>
+        <f t="shared" si="1"/>
+        <v>526.63199999999995</v>
       </c>
       <c r="H2" s="1">
-        <v>13.3</v>
+        <v>540.9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1136,389 +1262,569 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>469.56</v>
+        <v>790.39</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" si="0"/>
-        <v>483.82799999999997</v>
+        <v>821.428</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" si="0"/>
-        <v>498.096</v>
+        <f t="shared" si="1"/>
+        <v>852.46600000000001</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" si="0"/>
-        <v>512.36400000000003</v>
+        <f t="shared" si="1"/>
+        <v>883.50400000000002</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" si="0"/>
-        <v>526.63199999999995</v>
+        <f t="shared" si="1"/>
+        <v>914.54200000000003</v>
       </c>
       <c r="H3" s="1">
-        <v>540.9</v>
+        <v>945.58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>790.39</v>
+        <v>138.84</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>821.428</v>
+        <v>144.376</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="0"/>
-        <v>852.46600000000001</v>
+        <f t="shared" si="1"/>
+        <v>149.91200000000001</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>883.50400000000013</v>
+        <f t="shared" si="1"/>
+        <v>155.44800000000001</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="0"/>
-        <v>914.54199999999992</v>
+        <f t="shared" si="1"/>
+        <v>160.98400000000001</v>
       </c>
       <c r="H4" s="1">
-        <v>945.58</v>
+        <v>166.52</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4179</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>12</v>
       </c>
       <c r="C5" s="1">
-        <v>120.07</v>
+        <v>309.04000000000002</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>126.43199999999999</v>
+        <v>321.66200000000003</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="0"/>
-        <v>132.79399999999998</v>
+        <f t="shared" si="1"/>
+        <v>334.28399999999999</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>139.15600000000001</v>
+        <f t="shared" si="1"/>
+        <v>346.90600000000001</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="0"/>
-        <v>145.51799999999997</v>
+        <f t="shared" si="1"/>
+        <v>359.52799999999996</v>
       </c>
       <c r="H5" s="1">
-        <v>151.88</v>
+        <v>372.15</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>4179</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>24.36</v>
+        <v>144.41999999999999</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>25.635999999999999</v>
+        <v>146.47199999999998</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="0"/>
-        <v>26.911999999999995</v>
+        <f t="shared" si="1"/>
+        <v>148.524</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>28.188000000000002</v>
+        <f t="shared" si="1"/>
+        <v>150.57599999999999</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="0"/>
-        <v>29.463999999999995</v>
+        <f t="shared" si="1"/>
+        <v>152.62800000000001</v>
       </c>
       <c r="H6" s="1">
-        <v>30.74</v>
+        <v>154.68</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>4179</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1">
-        <v>5.73</v>
+        <v>359.72</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>6.008</v>
+        <v>388.77800000000002</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>6.2859999999999996</v>
+        <f t="shared" si="1"/>
+        <v>417.83600000000001</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="0"/>
-        <v>6.5640000000000009</v>
+        <f t="shared" si="1"/>
+        <v>446.89400000000001</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="0"/>
-        <v>6.8419999999999996</v>
+        <f t="shared" si="1"/>
+        <v>475.952</v>
       </c>
       <c r="H7" s="1">
-        <v>7.12</v>
+        <v>505.01</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
         <v>10</v>
       </c>
-      <c r="B8">
-        <v>4179</v>
-      </c>
       <c r="C8" s="1">
-        <v>4.18</v>
+        <v>73.19</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" ref="D8:D15" si="1">$C8+($H8-$C8)/($H7-$C7)*(D7-$C7)</f>
-        <v>4.3899999999999997</v>
+        <f t="shared" si="0"/>
+        <v>78.992000000000004</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" ref="E8:E15" si="2">$C8+($H8-$C8)/($H7-$C7)*(E7-$C7)</f>
-        <v>4.5999999999999996</v>
+        <f t="shared" si="1"/>
+        <v>84.793999999999997</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" ref="F8:F15" si="3">$C8+($H8-$C8)/($H7-$C7)*(F7-$C7)</f>
-        <v>4.8100000000000005</v>
+        <f t="shared" si="1"/>
+        <v>90.596000000000004</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ref="G8:G15" si="4">$C8+($H8-$C8)/($H7-$C7)*(G7-$C7)</f>
-        <v>5.0199999999999996</v>
+        <f t="shared" si="1"/>
+        <v>96.397999999999996</v>
       </c>
       <c r="H8" s="1">
-        <v>5.23</v>
+        <v>102.2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1">
-        <v>138.84</v>
+        <v>134.11000000000001</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="1"/>
-        <v>144.376</v>
+        <f t="shared" si="0"/>
+        <v>144.18600000000001</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="2"/>
-        <v>149.91200000000001</v>
+        <f t="shared" si="1"/>
+        <v>154.262</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="3"/>
-        <v>155.44800000000001</v>
+        <f t="shared" si="1"/>
+        <v>164.33800000000002</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="4"/>
-        <v>160.98399999999998</v>
+        <f t="shared" si="1"/>
+        <v>174.41400000000002</v>
       </c>
       <c r="H9" s="1">
-        <v>166.52</v>
+        <v>184.49</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>6</v>
+        <v>4525</v>
       </c>
       <c r="B10">
         <v>12</v>
       </c>
-      <c r="C10" s="1">
-        <v>309.04000000000002</v>
+      <c r="C10">
+        <v>60.034999999999997</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="1"/>
-        <v>321.66200000000003</v>
+        <f t="shared" si="0"/>
+        <v>63.215999999999994</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="2"/>
-        <v>334.28399999999999</v>
+        <f t="shared" si="1"/>
+        <v>66.396999999999991</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="3"/>
-        <v>346.90600000000001</v>
+        <f t="shared" si="1"/>
+        <v>69.578000000000003</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="4"/>
-        <v>359.52799999999991</v>
-      </c>
-      <c r="H10" s="1">
-        <v>372.15</v>
+        <f t="shared" si="1"/>
+        <v>72.759</v>
+      </c>
+      <c r="H10">
+        <v>75.94</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>6</v>
+        <v>3798</v>
       </c>
       <c r="B11">
-        <v>4179</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3.25</v>
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>60.034999999999997</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="1"/>
-        <v>3.3800000000000003</v>
+        <f t="shared" si="0"/>
+        <v>63.215999999999994</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="2"/>
-        <v>3.51</v>
+        <f t="shared" si="1"/>
+        <v>66.396999999999991</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="3"/>
-        <v>3.64</v>
+        <f t="shared" si="1"/>
+        <v>69.578000000000003</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="4"/>
-        <v>3.7699999999999991</v>
-      </c>
-      <c r="H11" s="1">
-        <v>3.9</v>
+        <f t="shared" si="1"/>
+        <v>72.759</v>
+      </c>
+      <c r="H11">
+        <v>75.94</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>6</v>
+        <v>4525</v>
       </c>
       <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1">
-        <v>144.41999999999999</v>
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>12.18</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="1"/>
-        <v>146.47200000000001</v>
+        <f t="shared" si="0"/>
+        <v>12.818</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="2"/>
-        <v>148.524</v>
+        <f t="shared" si="0"/>
+        <v>13.456</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="3"/>
-        <v>150.57599999999999</v>
+        <f t="shared" si="0"/>
+        <v>14.093999999999999</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="4"/>
-        <v>152.62799999999999</v>
-      </c>
-      <c r="H12" s="1">
-        <v>154.68</v>
+        <f t="shared" si="0"/>
+        <v>14.731999999999999</v>
+      </c>
+      <c r="H12">
+        <v>15.37</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2</v>
+        <v>3798</v>
       </c>
       <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1">
-        <v>359.72</v>
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>12.18</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="1"/>
-        <v>388.77800000000025</v>
+        <f t="shared" si="0"/>
+        <v>12.818</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="2"/>
-        <v>417.83600000000007</v>
+        <f t="shared" si="0"/>
+        <v>13.456</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="3"/>
-        <v>446.89399999999989</v>
+        <f t="shared" si="0"/>
+        <v>14.093999999999999</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="4"/>
-        <v>475.95199999999977</v>
-      </c>
-      <c r="H13" s="1">
-        <v>505.01</v>
+        <f t="shared" si="0"/>
+        <v>14.731999999999999</v>
+      </c>
+      <c r="H13">
+        <v>15.37</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2</v>
+        <v>4525</v>
       </c>
       <c r="B14">
-        <v>10</v>
-      </c>
-      <c r="C14" s="1">
-        <v>73.19</v>
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>2.8650000000000002</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="1"/>
-        <v>78.992000000000047</v>
+        <f t="shared" si="0"/>
+        <v>3.004</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="2"/>
-        <v>84.794000000000011</v>
+        <f t="shared" si="0"/>
+        <v>3.1430000000000002</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="3"/>
-        <v>90.595999999999975</v>
+        <f t="shared" si="0"/>
+        <v>3.282</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="4"/>
-        <v>96.397999999999954</v>
-      </c>
-      <c r="H14" s="1">
-        <v>102.2</v>
+        <f t="shared" si="0"/>
+        <v>3.4210000000000003</v>
+      </c>
+      <c r="H14">
+        <v>3.56</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>4</v>
+        <v>3798</v>
       </c>
       <c r="B15">
         <v>6</v>
       </c>
-      <c r="C15" s="1">
-        <v>134.11000000000001</v>
+      <c r="C15">
+        <v>2.8650000000000002</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="1"/>
-        <v>144.18600000000009</v>
+        <f t="shared" si="0"/>
+        <v>3.004</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="2"/>
-        <v>154.26200000000003</v>
+        <f t="shared" si="0"/>
+        <v>3.1430000000000002</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="3"/>
-        <v>164.33799999999997</v>
+        <f t="shared" si="0"/>
+        <v>3.282</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="4"/>
-        <v>174.41399999999993</v>
-      </c>
-      <c r="H15" s="1">
-        <v>184.49</v>
+        <f t="shared" si="0"/>
+        <v>3.4210000000000003</v>
+      </c>
+      <c r="H15">
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>4525</v>
+      </c>
+      <c r="C16">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>5.25</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>5.6000000000000005</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="0"/>
+        <v>5.95</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="0"/>
+        <v>6.3000000000000007</v>
+      </c>
+      <c r="H16">
+        <v>6.65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>3798</v>
+      </c>
+      <c r="C17">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>5.25</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>5.6000000000000005</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="0"/>
+        <v>5.95</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="0"/>
+        <v>6.3000000000000007</v>
+      </c>
+      <c r="H17">
+        <v>6.65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>4525</v>
+      </c>
+      <c r="C18">
+        <v>2.09</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1949999999999998</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4050000000000002</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5100000000000002</v>
+      </c>
+      <c r="H18">
+        <v>2.6150000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>3798</v>
+      </c>
+      <c r="C19">
+        <v>2.09</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1949999999999998</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4050000000000002</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5100000000000002</v>
+      </c>
+      <c r="H19">
+        <v>2.6150000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>4525</v>
+      </c>
+      <c r="C20">
+        <v>1.625</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>1.69</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7549999999999999</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="0"/>
+        <v>1.8199999999999998</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="0"/>
+        <v>1.885</v>
+      </c>
+      <c r="H20">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>3798</v>
+      </c>
+      <c r="C21">
+        <v>1.625</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>1.69</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7549999999999999</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="0"/>
+        <v>1.8199999999999998</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="0"/>
+        <v>1.885</v>
+      </c>
+      <c r="H21">
+        <v>1.95</v>
       </c>
     </row>
   </sheetData>
@@ -1528,10 +1834,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C15"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1552,10 +1858,10 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>4179</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>9.8000000000000007</v>
+        <v>469.56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1563,142 +1869,208 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>469.56</v>
+        <v>790.39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4">
-        <v>790.39</v>
+        <v>138.84</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4179</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>12</v>
       </c>
       <c r="C5">
-        <v>120.07</v>
+        <v>309.04000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>4179</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>24.36</v>
+        <v>144.41999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>4179</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>5.73</v>
+        <v>359.72</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
         <v>10</v>
       </c>
-      <c r="B8">
-        <v>4179</v>
-      </c>
       <c r="C8">
-        <v>4.18</v>
+        <v>73.19</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>138.84</v>
+        <v>134.11000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>6</v>
+        <v>4525</v>
       </c>
       <c r="B10">
         <v>12</v>
       </c>
       <c r="C10">
-        <v>309.04000000000002</v>
+        <v>60.034999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>6</v>
+        <v>3798</v>
       </c>
       <c r="B11">
-        <v>4179</v>
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>3.25</v>
+        <v>60.034999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>6</v>
+        <v>4525</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C12">
-        <v>144.41999999999999</v>
+        <v>12.18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2</v>
+        <v>3798</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <v>359.72</v>
+        <v>12.18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2</v>
+        <v>4525</v>
       </c>
       <c r="B14">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C14">
-        <v>73.19</v>
+        <v>2.8650000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>4</v>
+        <v>3798</v>
       </c>
       <c r="B15">
         <v>6</v>
       </c>
       <c r="C15">
-        <v>134.11000000000001</v>
+        <v>2.8650000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>4525</v>
+      </c>
+      <c r="C16">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>3798</v>
+      </c>
+      <c r="C17">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>4525</v>
+      </c>
+      <c r="C18">
+        <v>2.09</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>3798</v>
+      </c>
+      <c r="C19">
+        <v>2.09</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>4525</v>
+      </c>
+      <c r="C20">
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>3798</v>
+      </c>
+      <c r="C21">
+        <v>1.625</v>
       </c>
     </row>
   </sheetData>
@@ -1708,10 +2080,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1732,10 +2104,10 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>4179</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>13.3</v>
+        <v>540.9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1743,142 +2115,208 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>540.9</v>
+        <v>945.58</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4">
-        <v>945.58</v>
+        <v>166.52</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4179</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>12</v>
       </c>
       <c r="C5">
-        <v>151.88</v>
+        <v>372.15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>4179</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>30.74</v>
+        <v>154.68</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>4179</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>7.12</v>
+        <v>505.01</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
         <v>10</v>
       </c>
-      <c r="B8">
-        <v>4179</v>
-      </c>
       <c r="C8">
-        <v>5.23</v>
+        <v>102.2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>166.52</v>
+        <v>184.49</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>6</v>
+        <v>4525</v>
       </c>
       <c r="B10">
         <v>12</v>
       </c>
       <c r="C10">
-        <v>372.15</v>
+        <v>75.94</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>6</v>
+        <v>3798</v>
       </c>
       <c r="B11">
-        <v>4179</v>
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>3.9</v>
+        <v>75.94</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>6</v>
+        <v>4525</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C12">
-        <v>154.68</v>
+        <v>15.37</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2</v>
+        <v>3798</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <v>505.01</v>
+        <v>15.37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2</v>
+        <v>4525</v>
       </c>
       <c r="B14">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C14">
-        <v>102.2</v>
+        <v>3.56</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>4</v>
+        <v>3798</v>
       </c>
       <c r="B15">
         <v>6</v>
       </c>
       <c r="C15">
-        <v>184.49</v>
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>4525</v>
+      </c>
+      <c r="C16">
+        <v>6.65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>3798</v>
+      </c>
+      <c r="C17">
+        <v>6.65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>4525</v>
+      </c>
+      <c r="C18">
+        <v>2.6150000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>3798</v>
+      </c>
+      <c r="C19">
+        <v>2.6150000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>4525</v>
+      </c>
+      <c r="C20">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>3798</v>
+      </c>
+      <c r="C21">
+        <v>1.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>